<commit_message>
Se actualiza link de clases grabadas
</commit_message>
<xml_diff>
--- a/MaterialAdicional/ISW_2021_1C_LinksClasesGrabadas.xlsx
+++ b/MaterialAdicional/ISW_2021_1C_LinksClasesGrabadas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
   <si>
     <t>Día</t>
   </si>
@@ -325,13 +325,19 @@
     <t>Segundo Parcial</t>
   </si>
   <si>
-    <t>Comparación de enfoques tradicional, lean y agile</t>
-  </si>
-  <si>
-    <t>Deben traer para trabajar en clase un cuadro comparativo de los 3 enfoques (ver TP 14 en la guía de prácticos). Es evaluable</t>
+    <t>Retrospectiva</t>
+  </si>
+  <si>
+    <t>Deben traer para trabajar en clase un cuadro comparativo de los 3 enfoques (ver TP 14 en la guía de prácticos). Es evaluable. Se usará como recuperatorio de los TP conceptuales, para los grupos que lo necesiten</t>
+  </si>
+  <si>
+    <t>Clase Grabada Retrospectiva</t>
   </si>
   <si>
     <t>Publicidad en Instagram con herramientas de Design Thinking</t>
+  </si>
+  <si>
+    <t>Clase Grabada Practico 13</t>
   </si>
   <si>
     <t>Pecha Kucha</t>
@@ -361,6 +367,9 @@
       <t xml:space="preserve">
 https://youtu.be/u1bmaI4bEaU</t>
     </r>
+  </si>
+  <si>
+    <t>Clase Grabada Revisiones Tecnicas</t>
   </si>
   <si>
     <t>Recuperatorios</t>
@@ -521,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -579,6 +588,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -1366,7 +1378,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" ht="54.0" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -1377,13 +1389,15 @@
         <f t="shared" si="3"/>
         <v>44358</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="G28" s="7"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -1398,11 +1412,13 @@
         <v>44362</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="7"/>
+      <c r="G29" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
@@ -1415,8 +1431,8 @@
         <f t="shared" si="3"/>
         <v>44365</v>
       </c>
-      <c r="D30" s="27" t="s">
-        <v>74</v>
+      <c r="D30" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="3"/>
@@ -1434,15 +1450,17 @@
         <v>44369</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
@@ -1455,8 +1473,8 @@
         <f t="shared" si="3"/>
         <v>44372</v>
       </c>
-      <c r="D32" s="27" t="s">
-        <v>74</v>
+      <c r="D32" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="E32" s="3"/>
       <c r="G32" s="7"/>
@@ -1473,7 +1491,7 @@
         <v>44376</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E33" s="21"/>
       <c r="F33" s="3"/>
@@ -1491,15 +1509,15 @@
         <v>44379</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>82</v>
+      </c>
+      <c r="E34" s="28"/>
       <c r="F34" s="3"/>
       <c r="G34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="29"/>
-      <c r="E35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="E35" s="31"/>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
@@ -2498,11 +2516,14 @@
     <hyperlink r:id="rId19" ref="G22"/>
     <hyperlink r:id="rId20" ref="F24"/>
     <hyperlink r:id="rId21" ref="G25"/>
-    <hyperlink r:id="rId22" ref="F31"/>
+    <hyperlink r:id="rId22" ref="F28"/>
+    <hyperlink r:id="rId23" ref="G29"/>
+    <hyperlink r:id="rId24" ref="F31"/>
+    <hyperlink r:id="rId25" ref="G31"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId23"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>